<commit_message>
get all results and make latex tables
</commit_message>
<xml_diff>
--- a/Plotting/result_data_long.xlsx
+++ b/Plotting/result_data_long.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M123"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,7 +611,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Greenfield\Chemelot\20250422090637_2040_minC_DD10-1\optimization_results.h5</t>
+          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionLimit Greenfield\Chemelot\20250502092825_2040_minC_DD10-1\optimization_results.h5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionScope Greenfield\Chemelot\20250415015547_2040_minC_DD10-1\optimization_results.h5</t>
+          <t>Z:\AdOpt_NET0\AdOpt_results\MY\EmissionScope Greenfield\Chemelot\20250503162304_2040_minC_DD10-1\optimization_results.h5</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -675,7 +675,7 @@
         <v>4588155971.300325</v>
       </c>
       <c r="C6" t="n">
-        <v>4058616185.129568</v>
+        <v>4060745552.204102</v>
       </c>
       <c r="D6" t="n">
         <v>3327661021.24606</v>
@@ -693,7 +693,7 @@
         <v>4335623617.181549</v>
       </c>
       <c r="I6" t="n">
-        <v>3740341151.089449</v>
+        <v>3690001250.370417</v>
       </c>
       <c r="J6" t="n">
         <v>4145601469.212524</v>
@@ -776,7 +776,7 @@
         <v>137644679139.0098</v>
       </c>
       <c r="C9" t="n">
-        <v>121758485553.887</v>
+        <v>121822366566.1231</v>
       </c>
       <c r="D9" t="n">
         <v>99829830637.38179</v>
@@ -790,7 +790,7 @@
         <v>130068708515.4465</v>
       </c>
       <c r="I9" t="n">
-        <v>112210234532.6835</v>
+        <v>110700037511.1125</v>
       </c>
       <c r="J9" t="n">
         <v>124368044076.3757</v>
@@ -811,7 +811,7 @@
         <v>537986.8514076918</v>
       </c>
       <c r="C10" t="n">
-        <v>268993.4257000078</v>
+        <v>261268.6077500298</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -829,7 +829,7 @@
         <v>1585314.601209711</v>
       </c>
       <c r="I10" t="n">
-        <v>792657.3006048435</v>
+        <v>1062757.667</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -854,7 +854,7 @@
         <v>241.4597522945946</v>
       </c>
       <c r="C11" t="n">
-        <v>465.1666706762738</v>
+        <v>463.3378340998401</v>
       </c>
       <c r="D11" t="n">
         <v>190.6939783359936</v>
@@ -897,7 +897,7 @@
         <v>29.17470836460497</v>
       </c>
       <c r="C12" t="n">
-        <v>10.23851460762035</v>
+        <v>10.28347342169585</v>
       </c>
       <c r="D12" t="n">
         <v>27.9256466488213</v>
@@ -915,7 +915,7 @@
         <v>29.36413807663639</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1001290303683973</v>
+        <v>0.1025670297845189</v>
       </c>
       <c r="J12" t="n">
         <v>27.92665043793396</v>
@@ -940,7 +940,7 @@
         <v>65.3596136989397</v>
       </c>
       <c r="C13" t="n">
-        <v>138.9147767852318</v>
+        <v>139.4200441959811</v>
       </c>
       <c r="D13" t="n">
         <v>123.7363892061704</v>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>126.1411349876457</v>
+        <v>83.53193656506618</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -983,7 +983,7 @@
         <v>128.2926375707695</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1861040299176682</v>
+        <v>0.1867741364970346</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1001,7 +1001,7 @@
         <v>2.397682768479084</v>
       </c>
       <c r="I14" t="n">
-        <v>27.51773143172308</v>
+        <v>26.65051462965602</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>160.4369904663895</v>
+        <v>160.786378389205</v>
       </c>
       <c r="D15" t="n">
         <v>220.73212099268</v>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>92.16160502100482</v>
+        <v>53.98765915183444</v>
       </c>
       <c r="J15" t="n">
         <v>55.67753542372878</v>
@@ -1124,7 +1124,7 @@
         <v>496.8094804010865</v>
       </c>
       <c r="I17" t="n">
-        <v>305.5972325343301</v>
+        <v>295.8387604708937</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -1136,7 +1136,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>size_CrackerFurnace_Electric</t>
+          <t>size_CrackerFurnace_CC</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1148,15 +1148,9 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>0</v>
       </c>
@@ -1164,22 +1158,16 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>480.8519360653743</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>size_EDH</t>
+          <t>size_CrackerFurnace_Electric</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1207,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>480.8519360653743</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1222,20 +1210,20 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>size_ElectricSMR_m</t>
+          <t>size_EDH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>691.5746768003698</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>732.9997582129956</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>750.2247802366085</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1244,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>718.4745866438434</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1265,20 +1253,20 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>size_HBfeed_mixer</t>
+          <t>size_ElectricSMR_m</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>839.5599529382724</v>
+        <v>691.5746768003698</v>
       </c>
       <c r="C21" t="n">
-        <v>294.6335138883553</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>803.6157427006674</v>
+        <v>732.9997582129956</v>
       </c>
       <c r="E21" t="n">
-        <v>813</v>
+        <v>750.2247802366085</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1287,13 +1275,13 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>845.0111676729897</v>
+        <v>718.4745866438434</v>
       </c>
       <c r="I21" t="n">
-        <v>2.88141094585068</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>803.644616919011</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -1302,26 +1290,26 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>803.6205370246488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>size_HaberBosch</t>
+          <t>size_HBfeed_mixer</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>839.5599529382724</v>
       </c>
       <c r="C22" t="n">
-        <v>824.2886091158343</v>
+        <v>295.927292710672</v>
       </c>
       <c r="D22" t="n">
         <v>803.6157427006674</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>813</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1333,7 +1321,7 @@
         <v>845.0111676729897</v>
       </c>
       <c r="I22" t="n">
-        <v>806.2873059944878</v>
+        <v>2.951569202479543</v>
       </c>
       <c r="J22" t="n">
         <v>803.644616919011</v>
@@ -1345,26 +1333,26 @@
         <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>803.6205370246488</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>size_MPW2methanol</t>
+          <t>size_HaberBosch</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>338</v>
+        <v>839.5599529382724</v>
       </c>
       <c r="C23" t="n">
-        <v>328.0738354896167</v>
+        <v>827.48952215907</v>
       </c>
       <c r="D23" t="n">
-        <v>256.6658767599931</v>
+        <v>803.6157427006674</v>
       </c>
       <c r="E23" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1373,13 +1361,13 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>845.0111676729897</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>806.3173074331638</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>803.644616919011</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
@@ -1394,20 +1382,20 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>size_MTO</t>
+          <t>size_MPW2methanol</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>496.86</v>
+        <v>338</v>
       </c>
       <c r="C24" t="n">
-        <v>482.2685381697365</v>
+        <v>330.8595246788964</v>
       </c>
       <c r="D24" t="n">
-        <v>377.2988388371899</v>
+        <v>256.6658767599931</v>
       </c>
       <c r="E24" t="n">
-        <v>496.86</v>
+        <v>338</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1428,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>16.15068032936597</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
         <v>0</v>
@@ -1437,17 +1425,17 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>size_MeOHsynthesis</t>
+          <t>size_MPW2methanol_CC</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.3470064896086727</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.5803142409765671</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1471,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>19.62415592875574</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -1480,42 +1468,54 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>size_OlefinSeparation</t>
+          <t>size_MTO</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>496.86</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>486.3635012779777</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+        <v>377.2988388371899</v>
+      </c>
+      <c r="E26" t="n">
+        <v>496.86</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
       <c r="H26" t="n">
-        <v>496.8094804011101</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>305.5972325343301</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>480.851936065374</v>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>16.15068032936597</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>size_PDH</t>
+          <t>size_MeOHsynthesis</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>64.06277066356277</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>64.06277066356222</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1545,63 +1545,51 @@
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>139.4422956017326</v>
+        <v>19.62415592875574</v>
       </c>
       <c r="M27" t="n">
-        <v>62.22827334226069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>size_PE_mixer</t>
+          <t>size_OlefinSeparation</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>218</v>
-      </c>
-      <c r="E28" t="n">
-        <v>218</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>218</v>
+        <v>496.8094804011101</v>
       </c>
       <c r="I28" t="n">
-        <v>218</v>
+        <v>295.8387604708937</v>
       </c>
       <c r="J28" t="n">
-        <v>218</v>
-      </c>
-      <c r="K28" t="n">
-        <v>218</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
+        <v>480.851936065374</v>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>size_RWGS</t>
+          <t>size_PDH</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>64.06277066356277</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1610,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>64.06277066356222</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1631,81 +1619,93 @@
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>23.11443572291606</v>
+        <v>139.4422956017326</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>62.22827334226069</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>size_SteamReformer</t>
+          <t>size_PE_mixer</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="C30" t="n">
-        <v>695.9988110742169</v>
+        <v>218</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+        <v>218</v>
+      </c>
+      <c r="E30" t="n">
+        <v>218</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="I30" t="n">
-        <v>1055.738121448818</v>
+        <v>218</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
+        <v>218</v>
+      </c>
+      <c r="K30" t="n">
+        <v>218</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Ammonia</t>
+          <t>size_RWGS</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>7224.929599974984</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>5735.240118739349</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>135.1558286350344</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>4527.324722529889</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>4589.228877469824</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>8031.220348630261</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>1362.899133837197</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>76.10909367582423</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>28.51199999999994</v>
+        <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>1128.663540338653</v>
+        <v>23.11443572291606</v>
       </c>
       <c r="M31" t="n">
         <v>0</v>
@@ -1714,127 +1714,103 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Battery</t>
+          <t>size_SteamReformer</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1211.820683122364</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>5822.564647685514</v>
+        <v>698.5049007206281</v>
       </c>
       <c r="D32" t="n">
-        <v>1.223978279842899</v>
-      </c>
-      <c r="E32" t="n">
-        <v>1638.635814200616</v>
-      </c>
-      <c r="F32" t="n">
-        <v>6414</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>1338.884284164562</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>5031.024605684076</v>
+        <v>1055.671140907662</v>
       </c>
       <c r="J32" t="n">
-        <v>-9.620954020219218e-12</v>
-      </c>
-      <c r="K32" t="n">
-        <v>751.9801491116556</v>
-      </c>
-      <c r="L32" t="n">
-        <v>4350.515467440772</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_CO2</t>
+          <t>size_SteamReformer_CC</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>3863.466090635284</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>49.81125772464533</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>9813.150185612183</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>164.1639291732885</v>
+        <v>0.7307625331623093</v>
       </c>
       <c r="J33" t="n">
-        <v>-8.964411993122974e-11</v>
-      </c>
-      <c r="K33" t="n">
-        <v>6.654402102528422</v>
-      </c>
-      <c r="L33" t="n">
-        <v>4817.099911685627</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Ethylene</t>
+          <t>size_Storage_Ammonia</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>7224.929599974984</v>
       </c>
       <c r="C34" t="n">
-        <v>3273.6970139631</v>
+        <v>5628.724131190363</v>
       </c>
       <c r="D34" t="n">
-        <v>48.98932345440607</v>
+        <v>135.1558286350344</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>4527.324722529889</v>
       </c>
       <c r="F34" t="n">
-        <v>1365.207206316135</v>
+        <v>4589.228877469824</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>8031.220348630261</v>
       </c>
       <c r="I34" t="n">
-        <v>836.3574248818412</v>
+        <v>1396.31660880907</v>
       </c>
       <c r="J34" t="n">
-        <v>79.52372235661126</v>
+        <v>76.10909367582423</v>
       </c>
       <c r="K34" t="n">
-        <v>6.728399999930161</v>
+        <v>28.51199999999994</v>
       </c>
       <c r="L34" t="n">
-        <v>500</v>
+        <v>1128.663540338653</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
@@ -1843,41 +1819,41 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_H2</t>
+          <t>size_Storage_Battery</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>161.736827521127</v>
+        <v>1211.820683122364</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7170356792428301</v>
+        <v>5963.136299734941</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0005963225118775655</v>
+        <v>1.223978279842899</v>
       </c>
       <c r="E35" t="n">
-        <v>166.069363141339</v>
+        <v>1638.635814200616</v>
       </c>
       <c r="F35" t="n">
-        <v>8341.835870451305</v>
+        <v>6414</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>124.6378783694997</v>
+        <v>1338.884284164562</v>
       </c>
       <c r="I35" t="n">
-        <v>0.3954267082367138</v>
+        <v>4489.028038262079</v>
       </c>
       <c r="J35" t="n">
-        <v>-1.1032238324706e-10</v>
+        <v>-9.620954020219218e-12</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>751.9801491116556</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>4350.515467440772</v>
       </c>
       <c r="M35" t="n">
         <v>0</v>
@@ -1886,23 +1862,23 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Propylene</t>
+          <t>size_Storage_CO2</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>3020.962648652026</v>
+        <v>6460.904591607929</v>
       </c>
       <c r="D36" t="n">
-        <v>19.50685241530496</v>
+        <v>49.81125772464533</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>4448.725206689643</v>
+        <v>9813.150185612183</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -1911,16 +1887,16 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>9086.52802892159</v>
+        <v>41.16020129801905</v>
       </c>
       <c r="J36" t="n">
-        <v>130.6922726624625</v>
+        <v>-8.964411993122974e-11</v>
       </c>
       <c r="K36" t="n">
-        <v>5.767199999987153</v>
+        <v>6.654402102528422</v>
       </c>
       <c r="L36" t="n">
-        <v>9251.587161827001</v>
+        <v>4817.099911685627</v>
       </c>
       <c r="M36" t="n">
         <v>0</v>
@@ -1929,41 +1905,41 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>size_WGS_m</t>
+          <t>size_Storage_Ethylene</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>129.3244645616691</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>7112.261814987884</v>
       </c>
       <c r="D37" t="n">
-        <v>137.0709547858302</v>
+        <v>48.98932345440607</v>
       </c>
       <c r="E37" t="n">
-        <v>140.2920339042458</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>1365.207206316135</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>134.3547477023987</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>79.52372235661126</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>6.728399999930161</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M37" t="n">
         <v>0</v>
@@ -1972,41 +1948,41 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>size_feedgas_mixer</t>
+          <t>size_Storage_H2</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>802.7814448842365</v>
+        <v>161.736827521127</v>
       </c>
       <c r="C38" t="n">
-        <v>703.1849151041346</v>
+        <v>71.24392973672357</v>
       </c>
       <c r="D38" t="n">
-        <v>739.9997582129955</v>
+        <v>0.0005963225118775655</v>
       </c>
       <c r="E38" t="n">
-        <v>851.6175814425347</v>
+        <v>166.069363141339</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>8341.835870451305</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>725.4745866438434</v>
+        <v>124.6378783694997</v>
       </c>
       <c r="I38" t="n">
-        <v>1090.255852880541</v>
+        <v>0.5026247359710713</v>
       </c>
       <c r="J38" t="n">
-        <v>7</v>
+        <v>-1.1032238324706e-10</v>
       </c>
       <c r="K38" t="n">
-        <v>1119.63715986734</v>
+        <v>0</v>
       </c>
       <c r="L38" t="n">
-        <v>413.1272700336604</v>
+        <v>0</v>
       </c>
       <c r="M38" t="n">
         <v>0</v>
@@ -2015,23 +1991,23 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>size_naphtha_mixer</t>
+          <t>size_Storage_Propylene</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>571.2396212765573</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>19.50685241530496</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>4448.725206689643</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -2040,16 +2016,16 @@
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>8735.663655805742</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>130.6922726624625</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>5.767199999987153</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>9251.587161827001</v>
       </c>
       <c r="M39" t="n">
         <v>0</v>
@@ -2058,20 +2034,20 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>size_syngas_mixer</t>
+          <t>size_WGS_m</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>129.3244645616691</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>137.0709547858302</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>140.2920339042458</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -2080,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>134.3547477023987</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -2101,20 +2077,20 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>CO2/import_max</t>
+          <t>size_feedgas_mixer</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>802.7814448842365</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>705.6916748571251</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>739.9997582129955</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>851.6175814425347</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -2123,19 +2099,19 @@
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>725.4745866438434</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1089.321655537319</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>1119.63715986734</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>413.1272700336604</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
@@ -2144,41 +2120,41 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>CO2/export_max</t>
+          <t>size_naphtha_mixer</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>95.28244833291771</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>107.0945205148839</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>100.700063275586</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
         <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>82.93318857778478</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
@@ -2187,7 +2163,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>CO2_DAC/import_max</t>
+          <t>size_syngas_mixer</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2215,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>55.67753543597797</v>
+        <v>0</v>
       </c>
       <c r="K43" t="n">
         <v>0</v>
@@ -2224,13 +2200,13 @@
         <v>0</v>
       </c>
       <c r="M43" t="n">
-        <v>122.6813330321915</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>CO2_DAC/export_max</t>
+          <t>CO2/import_max</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2273,41 +2249,41 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>CO2captured/import_max</t>
+          <t>CO2/export_max</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>95.28244833291771</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>107.0945205148839</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>100.700063275586</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="L45" t="n">
-        <v>0</v>
+        <v>82.93318857778478</v>
       </c>
       <c r="M45" t="n">
         <v>0</v>
@@ -2316,7 +2292,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>CO2captured/export_max</t>
+          <t>CO2_DAC/import_max</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -2344,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>55.67753543597797</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
@@ -2353,13 +2329,13 @@
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>122.6813330321915</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>HBfeed/import_max</t>
+          <t>CO2_DAC/export_max</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -2402,7 +2378,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>HBfeed/export_max</t>
+          <t>CO2captured/import_max</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -2445,26 +2421,26 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>MPW/import_max</t>
+          <t>CO2captured/export_max</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>328.0738354896167</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>256.6658767599931</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>338</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -2488,7 +2464,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>MPW/export_max</t>
+          <t>HBfeed/import_max</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2531,7 +2507,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>PE_olefin/import_max</t>
+          <t>HBfeed/export_max</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -2574,26 +2550,26 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>PE_olefin/export_max</t>
+          <t>MPW/import_max</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>330.8595246789071</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>256.6658767599931</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -2617,7 +2593,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>ammonia/import_max</t>
+          <t>MPW/export_max</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2660,7 +2636,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>ammonia/export_max</t>
+          <t>PE_olefin/import_max</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2703,7 +2679,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>crackergas/import_max</t>
+          <t>PE_olefin/export_max</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -2746,7 +2722,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>crackergas/export_max</t>
+          <t>ammonia/import_max</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -2768,13 +2744,13 @@
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>91.22068676723228</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>372.1453988827569</v>
+        <v>0</v>
       </c>
       <c r="K56" t="n">
         <v>0</v>
@@ -2789,50 +2765,50 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>electricity/import_max</t>
+          <t>ammonia/export_max</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>2500.000004299729</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>2500.000000001289</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>2500.000000007237</v>
+        <v>0</v>
       </c>
       <c r="K57" t="n">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="M57" t="n">
-        <v>2500.000000007921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>electricity/export_max</t>
+          <t>crackergas/import_max</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -2875,7 +2851,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>ethanol/import_max</t>
+          <t>crackergas/export_max</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -2897,13 +2873,13 @@
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>91.22068676723228</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>0</v>
+        <v>372.1453988827569</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
@@ -2918,50 +2894,50 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>ethanol/export_max</t>
+          <t>electricity/import_max</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>2500.000004299729</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>2500.000000001289</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="J60" t="n">
-        <v>0</v>
+        <v>2500.000000007237</v>
       </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="L60" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="M60" t="n">
-        <v>0</v>
+        <v>2500.000000007921</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>ethylene/import_max</t>
+          <t>electricity/export_max</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -3004,7 +2980,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>ethylene/export_max</t>
+          <t>ethanol/import_max</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3047,7 +3023,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>feedgas/import_max</t>
+          <t>ethanol/export_max</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3090,7 +3066,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>feedgas/export_max</t>
+          <t>ethylene/import_max</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3133,7 +3109,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>heatlowT/import_max</t>
+          <t>ethylene/export_max</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3176,35 +3152,35 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>heatlowT/export_max</t>
+          <t>feedgas/import_max</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>39.35793962401891</v>
+        <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>75.82216732023264</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>31.08311857282024</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>22.9051186366608</v>
+        <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>44.69727137654262</v>
+        <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>44.69727137654262</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>46.07678054854758</v>
+        <v>0</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>208.200170478013</v>
+        <v>0</v>
       </c>
       <c r="K66" t="n">
         <v>0</v>
@@ -3213,13 +3189,13 @@
         <v>0</v>
       </c>
       <c r="M66" t="n">
-        <v>167.3191848842364</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>hydrogen/import_max</t>
+          <t>feedgas/export_max</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3262,7 +3238,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>hydrogen/export_max</t>
+          <t>heatlowT/import_max</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -3305,50 +3281,50 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>methane/import_max</t>
+          <t>heatlowT/export_max</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>802.7814448843585</v>
+        <v>39.35793962401891</v>
       </c>
       <c r="C69" t="n">
-        <v>703.1849151041346</v>
+        <v>75.52406695827393</v>
       </c>
       <c r="D69" t="n">
-        <v>739.9997598422402</v>
+        <v>31.08311857282024</v>
       </c>
       <c r="E69" t="n">
-        <v>851.6175814425347</v>
+        <v>22.9051186366608</v>
       </c>
       <c r="F69" t="n">
-        <v>757.2247802366086</v>
+        <v>44.69727137654262</v>
       </c>
       <c r="G69" t="n">
-        <v>757.2247802366086</v>
+        <v>44.69727137654262</v>
       </c>
       <c r="H69" t="n">
-        <v>337.4663824510857</v>
+        <v>46.07678054854758</v>
       </c>
       <c r="I69" t="n">
-        <v>851.5844142712293</v>
+        <v>0</v>
       </c>
       <c r="J69" t="n">
-        <v>3.600036815699374</v>
+        <v>208.200170478013</v>
       </c>
       <c r="K69" t="n">
-        <v>733.9114905600854</v>
+        <v>0</v>
       </c>
       <c r="L69" t="n">
-        <v>1532.764429901001</v>
+        <v>0</v>
       </c>
       <c r="M69" t="n">
-        <v>7</v>
+        <v>167.3191848842364</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>methane/export_max</t>
+          <t>hydrogen/import_max</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -3391,7 +3367,7 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>methane_bio/import_max</t>
+          <t>hydrogen/export_max</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -3434,50 +3410,50 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>methane_bio/export_max</t>
+          <t>methane/import_max</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>802.7814448843585</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>705.6916748571488</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>739.9997598422402</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>851.6175814425347</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>757.2247802366086</v>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>757.2247802366086</v>
       </c>
       <c r="H72" t="n">
-        <v>0</v>
+        <v>337.4663824510857</v>
       </c>
       <c r="I72" t="n">
-        <v>0</v>
+        <v>858.271583609551</v>
       </c>
       <c r="J72" t="n">
-        <v>0</v>
+        <v>3.600036815699374</v>
       </c>
       <c r="K72" t="n">
-        <v>0</v>
+        <v>733.9114905600854</v>
       </c>
       <c r="L72" t="n">
-        <v>0</v>
+        <v>1532.764429901001</v>
       </c>
       <c r="M72" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>methanol/import_max</t>
+          <t>methane/export_max</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -3520,7 +3496,7 @@
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>methanol/export_max</t>
+          <t>methane_bio/import_max</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -3563,7 +3539,7 @@
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
-          <t>naphtha/import_max</t>
+          <t>methane_bio/export_max</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3585,16 +3561,16 @@
         <v>0</v>
       </c>
       <c r="H75" t="n">
-        <v>496.8094804014871</v>
+        <v>0</v>
       </c>
       <c r="I75" t="n">
-        <v>305.5972325343301</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>480.8519360653744</v>
+        <v>0</v>
       </c>
       <c r="K75" t="n">
-        <v>499</v>
+        <v>0</v>
       </c>
       <c r="L75" t="n">
         <v>0</v>
@@ -3606,7 +3582,7 @@
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
         <is>
-          <t>naphtha/export_max</t>
+          <t>methanol/import_max</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3649,7 +3625,7 @@
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>naphtha_bio/import_max</t>
+          <t>methanol/export_max</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3692,7 +3668,7 @@
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>naphtha_bio/export_max</t>
+          <t>naphtha/import_max</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -3714,16 +3690,16 @@
         <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>0</v>
+        <v>496.8094804014871</v>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>295.8387604708937</v>
       </c>
       <c r="J78" t="n">
-        <v>0</v>
+        <v>480.8519360653744</v>
       </c>
       <c r="K78" t="n">
-        <v>0</v>
+        <v>499</v>
       </c>
       <c r="L78" t="n">
         <v>0</v>
@@ -3735,7 +3711,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>nitrogen/import_max</t>
+          <t>naphtha/export_max</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -3778,14 +3754,14 @@
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>nitrogen/export_max</t>
+          <t>naphtha_bio/import_max</t>
         </is>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>24.56951476961811</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
@@ -3803,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="n">
-        <v>0.2974037375105262</v>
+        <v>0</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
@@ -3821,7 +3797,7 @@
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
         <is>
-          <t>olefins/import_max</t>
+          <t>naphtha_bio/export_max</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -3864,7 +3840,7 @@
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>olefins/export_max</t>
+          <t>nitrogen/import_max</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -3907,14 +3883,14 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>oxygen/import_max</t>
+          <t>nitrogen/export_max</t>
         </is>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>24.68033621209661</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
@@ -3932,7 +3908,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>0.3282144953105938</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
@@ -3950,35 +3926,35 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>oxygen/export_max</t>
+          <t>olefins/import_max</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>71.77487025526489</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>81.87249135431496</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>62.67817180838598</v>
+        <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>55.60270508351208</v>
+        <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>75.52313918315861</v>
+        <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>75.52313918315859</v>
+        <v>0</v>
       </c>
       <c r="H84" t="n">
-        <v>78.14906307484014</v>
+        <v>0</v>
       </c>
       <c r="I84" t="n">
-        <v>0.1228583202682043</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>224.5839473341176</v>
+        <v>0</v>
       </c>
       <c r="K84" t="n">
         <v>0</v>
@@ -3987,26 +3963,26 @@
         <v>0</v>
       </c>
       <c r="M84" t="n">
-        <v>187.2131853144176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>propane/import_max</t>
+          <t>olefins/export_max</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>64.06277066385512</v>
+        <v>0</v>
       </c>
       <c r="C85" t="n">
         <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>9.828169869926391e-07</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>64.06277066385586</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -4027,16 +4003,16 @@
         <v>0</v>
       </c>
       <c r="L85" t="n">
-        <v>139.4422956022084</v>
+        <v>0</v>
       </c>
       <c r="M85" t="n">
-        <v>201.6705689439933</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>propane/export_max</t>
+          <t>oxygen/import_max</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -4079,35 +4055,35 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>propylene/import_max</t>
+          <t>oxygen/export_max</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>71.77487025526489</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>81.65515916929698</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>62.67817180838598</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>55.60270508351208</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>75.52313918315861</v>
       </c>
       <c r="G87" t="n">
-        <v>0</v>
+        <v>75.52313918315859</v>
       </c>
       <c r="H87" t="n">
-        <v>0</v>
+        <v>78.14906307484014</v>
       </c>
       <c r="I87" t="n">
-        <v>0</v>
+        <v>0.1258497455519617</v>
       </c>
       <c r="J87" t="n">
-        <v>0</v>
+        <v>224.5839473341176</v>
       </c>
       <c r="K87" t="n">
         <v>0</v>
@@ -4116,26 +4092,26 @@
         <v>0</v>
       </c>
       <c r="M87" t="n">
-        <v>0</v>
+        <v>187.2131853144176</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>propylene/export_max</t>
+          <t>propane/import_max</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>64.06277066385512</v>
       </c>
       <c r="C88" t="n">
         <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>9.828169869926391e-07</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>64.06277066385586</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -4156,16 +4132,16 @@
         <v>0</v>
       </c>
       <c r="L88" t="n">
-        <v>0</v>
+        <v>139.4422956022084</v>
       </c>
       <c r="M88" t="n">
-        <v>0</v>
+        <v>201.6705689439933</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>steam/import_max</t>
+          <t>propane/export_max</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -4208,7 +4184,7 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>steam/export_max</t>
+          <t>propylene/import_max</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -4218,25 +4194,25 @@
         <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>4.180236601314391e-08</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>92.682</v>
+        <v>0</v>
       </c>
       <c r="G90" t="n">
         <v>0</v>
       </c>
       <c r="H90" t="n">
-        <v>55.59289572185796</v>
+        <v>0</v>
       </c>
       <c r="I90" t="n">
         <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>115.6580831321342</v>
+        <v>0</v>
       </c>
       <c r="K90" t="n">
         <v>0</v>
@@ -4251,7 +4227,7 @@
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>syngas/import_max</t>
+          <t>propylene/export_max</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -4294,7 +4270,7 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>syngas/export_max</t>
+          <t>steam/import_max</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -4337,35 +4313,35 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>syngas_r/import_max</t>
+          <t>steam/export_max</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>7.949975784409219</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>4.180236601314391e-08</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
+        <v>92.682</v>
       </c>
       <c r="G93" t="n">
         <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>0</v>
+        <v>55.59289572185796</v>
       </c>
       <c r="I93" t="n">
         <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>0</v>
+        <v>115.6580831321342</v>
       </c>
       <c r="K93" t="n">
         <v>0</v>
@@ -4380,7 +4356,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>syngas_r/export_max</t>
+          <t>syngas/import_max</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -4423,33 +4399,41 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>size_CO2electrolysis</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
+          <t>syngas/export_max</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
       <c r="C95" t="n">
-        <v>106.4562506298236</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>156.575247234887</v>
-      </c>
-      <c r="E95" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
       <c r="F95" t="n">
-        <v>111.1724125179555</v>
+        <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>39.78106601603671</v>
-      </c>
-      <c r="H95" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
       <c r="I95" t="n">
-        <v>151.6294897513077</v>
+        <v>0</v>
       </c>
       <c r="J95" t="n">
-        <v>11.67753542373834</v>
-      </c>
-      <c r="K95" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
       <c r="L95" t="n">
-        <v>161.3511675354761</v>
+        <v>0</v>
       </c>
       <c r="M95" t="n">
         <v>0</v>
@@ -4458,31 +4442,39 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>size_DirectMeOHsynthesis</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr"/>
+          <t>syngas_r/import_max</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
       <c r="C96" t="n">
         <v>0</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
       <c r="F96" t="n">
         <v>0</v>
       </c>
       <c r="G96" t="n">
         <v>0</v>
       </c>
-      <c r="H96" t="inlineStr"/>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
       <c r="I96" t="n">
         <v>0</v>
       </c>
       <c r="J96" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr"/>
+      <c r="K96" t="n">
+        <v>0</v>
+      </c>
       <c r="L96" t="n">
         <v>0</v>
       </c>
@@ -4493,88 +4485,120 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>size_CrackerFurnace_existing</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
+          <t>syngas_r/export_max</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
       <c r="E97" t="n">
         <v>0</v>
       </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
-      <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0</v>
+      </c>
       <c r="K97" t="n">
-        <v>499</v>
+        <v>0</v>
       </c>
       <c r="L97" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr"/>
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>size_HaberBosch_existing</t>
+          <t>size_CO2electrolysis</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="n">
-        <v>813</v>
-      </c>
+      <c r="C98" t="n">
+        <v>106.4070678571697</v>
+      </c>
+      <c r="D98" t="n">
+        <v>156.575247234887</v>
+      </c>
+      <c r="E98" t="inlineStr"/>
       <c r="F98" t="n">
-        <v>813</v>
+        <v>111.1724125179555</v>
       </c>
       <c r="G98" t="n">
-        <v>813</v>
+        <v>39.78106601603671</v>
       </c>
       <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="n">
-        <v>813</v>
-      </c>
+      <c r="I98" t="n">
+        <v>155.3457474964666</v>
+      </c>
+      <c r="J98" t="n">
+        <v>11.67753542373834</v>
+      </c>
+      <c r="K98" t="inlineStr"/>
       <c r="L98" t="n">
-        <v>813</v>
+        <v>161.3511675354761</v>
       </c>
       <c r="M98" t="n">
-        <v>813</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>size_OlefinSeparation_existing</t>
+          <t>size_DirectMeOHsynthesis</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="n">
-        <v>0</v>
-      </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
       <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr"/>
-      <c r="K99" t="n">
-        <v>499</v>
-      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr"/>
       <c r="L99" t="n">
         <v>0</v>
       </c>
-      <c r="M99" t="inlineStr"/>
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>size_SteamReformer_existing</t>
+          <t>size_CrackerFurnace_existing</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -4589,142 +4613,152 @@
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="n">
-        <v>1078</v>
+        <v>499</v>
       </c>
       <c r="L100" t="n">
-        <v>1078</v>
-      </c>
-      <c r="M100" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>size_AEC_existing</t>
+          <t>size_CrackerFurnace_existing_CC</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="n">
-        <v>140.5222002249128</v>
-      </c>
-      <c r="G101" t="n">
-        <v>274.2163888131449</v>
-      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
+      <c r="K101" t="n">
+        <v>0</v>
+      </c>
+      <c r="L101" t="n">
+        <v>0</v>
+      </c>
       <c r="M101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>size_ASU_existing</t>
+          <t>size_HaberBosch_existing</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
+      <c r="E102" t="n">
+        <v>813</v>
+      </c>
       <c r="F102" t="n">
-        <v>28.25175</v>
+        <v>813</v>
       </c>
       <c r="G102" t="n">
-        <v>28.25175</v>
+        <v>813</v>
       </c>
       <c r="H102" t="inlineStr"/>
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr"/>
-      <c r="K102" t="inlineStr"/>
-      <c r="L102" t="inlineStr"/>
-      <c r="M102" t="inlineStr"/>
+      <c r="K102" t="n">
+        <v>813</v>
+      </c>
+      <c r="L102" t="n">
+        <v>813</v>
+      </c>
+      <c r="M102" t="n">
+        <v>813</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>size_Boiler_El_existing</t>
+          <t>size_OlefinSeparation_existing</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
-      <c r="F103" t="n">
-        <v>64.27389941323595</v>
-      </c>
-      <c r="G103" t="n">
-        <v>64.27389941323595</v>
-      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr"/>
-      <c r="K103" t="inlineStr"/>
+      <c r="K103" t="n">
+        <v>499</v>
+      </c>
       <c r="L103" t="n">
-        <v>41.59677723356639</v>
-      </c>
-      <c r="M103" t="n">
-        <v>41.59677723356639</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>size_Boiler_Industrial_NG_existing</t>
+          <t>size_SteamReformer_existing</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
-      <c r="F104" t="n">
-        <v>124.7900274942034</v>
-      </c>
-      <c r="G104" t="n">
-        <v>124.7900274942034</v>
-      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr"/>
+      <c r="K104" t="n">
+        <v>1078</v>
+      </c>
       <c r="L104" t="n">
-        <v>44.30601663477577</v>
+        <v>1078</v>
       </c>
       <c r="M104" t="n">
-        <v>457.4332866684121</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>size_ElectricSMR_m_existing</t>
+          <t>size_SteamReformer_existing_CC</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
-      <c r="F105" t="n">
-        <v>750.2247802366085</v>
-      </c>
-      <c r="G105" t="n">
-        <v>750.2247802366085</v>
-      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr"/>
-      <c r="L105" t="inlineStr"/>
-      <c r="M105" t="inlineStr"/>
+      <c r="K105" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" t="n">
+        <v>0.8799542698396018</v>
+      </c>
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>size_HBfeed_mixer_existing</t>
+          <t>size_AEC_existing</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -4732,10 +4766,10 @@
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="n">
-        <v>813</v>
+        <v>140.5222002249128</v>
       </c>
       <c r="G106" t="n">
-        <v>813</v>
+        <v>274.2163888131449</v>
       </c>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
@@ -4747,7 +4781,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>size_MPW2methanol_existing</t>
+          <t>size_ASU_existing</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -4755,10 +4789,10 @@
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="n">
-        <v>338</v>
+        <v>28.25175</v>
       </c>
       <c r="G107" t="n">
-        <v>338</v>
+        <v>28.25175</v>
       </c>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
@@ -4770,7 +4804,7 @@
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>size_MTO_existing</t>
+          <t>size_Boiler_El_existing</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -4778,24 +4812,26 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="n">
-        <v>496.86</v>
+        <v>64.27389941323595</v>
       </c>
       <c r="G108" t="n">
-        <v>496.86</v>
+        <v>64.27389941323595</v>
       </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
-      <c r="L108" t="inlineStr"/>
+      <c r="L108" t="n">
+        <v>41.59677723356639</v>
+      </c>
       <c r="M108" t="n">
-        <v>16.15068032936597</v>
+        <v>41.59677723356639</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>size_PDH_existing</t>
+          <t>size_Boiler_Industrial_NG_existing</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -4803,24 +4839,26 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="n">
-        <v>64.06277066356222</v>
+        <v>124.7900274942034</v>
       </c>
       <c r="G109" t="n">
-        <v>64.06277066356222</v>
+        <v>124.7900274942034</v>
       </c>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
-      <c r="L109" t="inlineStr"/>
+      <c r="L109" t="n">
+        <v>44.30601663477577</v>
+      </c>
       <c r="M109" t="n">
-        <v>139.4422956017326</v>
+        <v>457.4332866684121</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>size_PE_mixer_existing</t>
+          <t>size_ElectricSMR_m_existing</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -4828,26 +4866,22 @@
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="n">
-        <v>218</v>
+        <v>750.2247802366085</v>
       </c>
       <c r="G110" t="n">
-        <v>218</v>
+        <v>750.2247802366085</v>
       </c>
       <c r="H110" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
-      <c r="L110" t="n">
-        <v>218</v>
-      </c>
-      <c r="M110" t="n">
-        <v>218</v>
-      </c>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Ammonia_existing</t>
+          <t>size_HBfeed_mixer_existing</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -4855,26 +4889,22 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="n">
-        <v>4527.324722529889</v>
+        <v>813</v>
       </c>
       <c r="G111" t="n">
-        <v>9116.553599999712</v>
+        <v>813</v>
       </c>
       <c r="H111" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
-      <c r="L111" t="n">
-        <v>28.51199999999994</v>
-      </c>
-      <c r="M111" t="n">
-        <v>1157.175540338653</v>
-      </c>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Battery_existing</t>
+          <t>size_MPW2methanol_existing</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -4882,26 +4912,22 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="n">
-        <v>1638.635814200616</v>
+        <v>338</v>
       </c>
       <c r="G112" t="n">
-        <v>8052.635814200616</v>
+        <v>338</v>
       </c>
       <c r="H112" t="inlineStr"/>
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
-      <c r="L112" t="n">
-        <v>751.9801491116556</v>
-      </c>
-      <c r="M112" t="n">
-        <v>5102.495616552428</v>
-      </c>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_H2_existing</t>
+          <t>size_MPW2methanol_existing_CC</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -4909,10 +4935,10 @@
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="n">
-        <v>166.069363141339</v>
+        <v>0.2901160949630602</v>
       </c>
       <c r="G113" t="n">
-        <v>8507.905233592644</v>
+        <v>0.5309751217410748</v>
       </c>
       <c r="H113" t="inlineStr"/>
       <c r="I113" t="inlineStr"/>
@@ -4924,7 +4950,7 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>size_WGS_m_existing</t>
+          <t>size_MTO_existing</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -4932,22 +4958,24 @@
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="n">
-        <v>140.2920339042458</v>
+        <v>496.86</v>
       </c>
       <c r="G114" t="n">
-        <v>140.2920339042458</v>
+        <v>496.86</v>
       </c>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
-      <c r="M114" t="inlineStr"/>
+      <c r="M114" t="n">
+        <v>16.15068032936597</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>size_feedgas_mixer_existing</t>
+          <t>size_PDH_existing</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -4955,170 +4983,178 @@
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="n">
-        <v>851.6175814425347</v>
+        <v>64.06277066356222</v>
       </c>
       <c r="G115" t="n">
-        <v>851.6175814425347</v>
+        <v>64.06277066356222</v>
       </c>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
-      <c r="L115" t="n">
-        <v>1119.63715986734</v>
-      </c>
+      <c r="L115" t="inlineStr"/>
       <c r="M115" t="n">
-        <v>1532.764429901001</v>
+        <v>139.4422956017326</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>size_CO2_mixer_existing</t>
+          <t>size_PE_mixer_existing</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
-      <c r="F116" t="inlineStr"/>
+      <c r="F116" t="n">
+        <v>218</v>
+      </c>
       <c r="G116" t="n">
-        <v>129.5851882841922</v>
+        <v>218</v>
       </c>
       <c r="H116" t="inlineStr"/>
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
-      <c r="L116" t="inlineStr"/>
+      <c r="L116" t="n">
+        <v>218</v>
+      </c>
       <c r="M116" t="n">
-        <v>63.76725947358676</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>size_CO2electrolysis_existing</t>
+          <t>size_Storage_Ammonia_existing</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
-      <c r="F117" t="inlineStr"/>
+      <c r="F117" t="n">
+        <v>4527.324722529889</v>
+      </c>
       <c r="G117" t="n">
-        <v>111.1724125179555</v>
+        <v>9116.553599999712</v>
       </c>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
-      <c r="L117" t="inlineStr"/>
+      <c r="L117" t="n">
+        <v>28.51199999999994</v>
+      </c>
       <c r="M117" t="n">
-        <v>161.3511675354761</v>
+        <v>1157.175540338653</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_CO2_existing</t>
+          <t>size_Storage_Battery_existing</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
-      <c r="F118" t="inlineStr"/>
+      <c r="F118" t="n">
+        <v>1638.635814200616</v>
+      </c>
       <c r="G118" t="n">
-        <v>9813.150185612183</v>
+        <v>8052.635814200616</v>
       </c>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr"/>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="n">
-        <v>6.654402102528422</v>
+        <v>751.9801491116556</v>
       </c>
       <c r="M118" t="n">
-        <v>4823.754313788156</v>
+        <v>5102.495616552428</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Ethylene_existing</t>
+          <t>size_Storage_H2_existing</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
-      <c r="F119" t="inlineStr"/>
+      <c r="F119" t="n">
+        <v>166.069363141339</v>
+      </c>
       <c r="G119" t="n">
-        <v>1365.207206316135</v>
+        <v>8507.905233592644</v>
       </c>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
-      <c r="L119" t="n">
-        <v>6.728399999930161</v>
-      </c>
-      <c r="M119" t="n">
-        <v>506.7283999999302</v>
-      </c>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>size_Storage_Propylene_existing</t>
+          <t>size_WGS_m_existing</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
       <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
-      <c r="F120" t="inlineStr"/>
+      <c r="F120" t="n">
+        <v>140.2920339042458</v>
+      </c>
       <c r="G120" t="n">
-        <v>4448.725206689643</v>
+        <v>140.2920339042458</v>
       </c>
       <c r="H120" t="inlineStr"/>
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
-      <c r="L120" t="n">
-        <v>5.767199999987153</v>
-      </c>
-      <c r="M120" t="n">
-        <v>9257.354361826989</v>
-      </c>
+      <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>size_CO2toEmission_existing</t>
+          <t>size_feedgas_mixer_existing</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
+      <c r="F121" t="n">
+        <v>851.6175814425347</v>
+      </c>
+      <c r="G121" t="n">
+        <v>851.6175814425347</v>
+      </c>
       <c r="H121" t="inlineStr"/>
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="n">
-        <v>6.522996057621048</v>
+        <v>1119.63715986734</v>
       </c>
       <c r="M121" t="n">
-        <v>6.522996057621048</v>
+        <v>1532.764429901001</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>size_MeOHsynthesis_existing</t>
+          <t>size_CO2_mixer_existing</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -5126,20 +5162,22 @@
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
-      <c r="G122" t="inlineStr"/>
+      <c r="G122" t="n">
+        <v>129.5851882841922</v>
+      </c>
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
       <c r="M122" t="n">
-        <v>19.62415592875574</v>
+        <v>63.76725947358676</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>size_RWGS_existing</t>
+          <t>size_CO2electrolysis_existing</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -5147,13 +5185,155 @@
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
-      <c r="G123" t="inlineStr"/>
+      <c r="G123" t="n">
+        <v>111.1724125179555</v>
+      </c>
       <c r="H123" t="inlineStr"/>
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
       <c r="M123" t="n">
+        <v>161.3511675354761</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>size_Storage_CO2_existing</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr"/>
+      <c r="G124" t="n">
+        <v>9813.150185612183</v>
+      </c>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" t="n">
+        <v>6.654402102528422</v>
+      </c>
+      <c r="M124" t="n">
+        <v>4823.754313788156</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>size_Storage_Ethylene_existing</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr"/>
+      <c r="G125" t="n">
+        <v>1365.207206316135</v>
+      </c>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
+      <c r="K125" t="inlineStr"/>
+      <c r="L125" t="n">
+        <v>6.728399999930161</v>
+      </c>
+      <c r="M125" t="n">
+        <v>506.7283999999302</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>size_Storage_Propylene_existing</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr"/>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr"/>
+      <c r="G126" t="n">
+        <v>4448.725206689643</v>
+      </c>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" t="n">
+        <v>5.767199999987153</v>
+      </c>
+      <c r="M126" t="n">
+        <v>9257.354361826989</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>size_CO2toEmission_existing</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
+      <c r="K127" t="inlineStr"/>
+      <c r="L127" t="n">
+        <v>6.522996057621048</v>
+      </c>
+      <c r="M127" t="n">
+        <v>6.522996057621048</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>size_MeOHsynthesis_existing</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
+      <c r="L128" t="inlineStr"/>
+      <c r="M128" t="n">
+        <v>19.62415592875574</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>size_RWGS_existing</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
+      <c r="L129" t="inlineStr"/>
+      <c r="M129" t="n">
         <v>23.11443572291606</v>
       </c>
     </row>

</xml_diff>